<commit_message>
reproduction data collection complete
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Creature Traits" sheetId="1" r:id="rId1"/>
@@ -23,15 +23,15 @@
     <sheet name="Environment" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="c_avgs_1" localSheetId="1">'Creature Averages'!$A$1:$L$2</definedName>
-    <definedName name="c_traits_1" localSheetId="0">'Creature Traits'!$A$1:$M$36</definedName>
+    <definedName name="c_avgs" localSheetId="1">'Creature Averages'!$A$1:$L$3</definedName>
+    <definedName name="c_traits_1" localSheetId="0">'Creature Traits'!$A$1:$M$43</definedName>
     <definedName name="env_1" localSheetId="8">Environment!$A$1:$L$2</definedName>
     <definedName name="lifetime_1" localSheetId="5">'Lifetime ticks'!$A$1:$F$2</definedName>
-    <definedName name="metabolism" localSheetId="4">Metabolism!$A$1:$L$2</definedName>
+    <definedName name="metabolism_1" localSheetId="4">Metabolism!$A$1:$L$43</definedName>
     <definedName name="p_impact_1" localSheetId="6">'Player Impact'!$A$1:$F$2</definedName>
     <definedName name="p_stats" localSheetId="7">'Player Stats'!$A$1:$P$2</definedName>
-    <definedName name="reproduction_1" localSheetId="2">'Reproductive Traits'!$A$1:$G$2</definedName>
-    <definedName name="sensing_1" localSheetId="3">Sensing!$A$1:$D$2</definedName>
+    <definedName name="reproduction" localSheetId="2">'Reproductive Traits'!$A$1:$G$43</definedName>
+    <definedName name="sensing" localSheetId="3">Sensing!$A$1:$D$43</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -276,9 +276,6 @@
     <t xml:space="preserve">   Gamete Cost   </t>
   </si>
   <si>
-    <t xml:space="preserve">   Spawn Time   </t>
-  </si>
-  <si>
     <t xml:space="preserve">   Creature Scent   </t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t xml:space="preserve">   Overall Lightning Accuracy   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Gamete Time   </t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -536,11 +536,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,6 +624,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,19 +651,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="c_avgs_1" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="c_avgs" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reproduction_1" refreshOnLoad="1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="reproduction" refreshOnLoad="1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sensing_1" refreshOnLoad="1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sensing" refreshOnLoad="1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="metabolism" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="metabolism_1" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -898,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,19 +1017,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="18">
-        <v>118.44893</v>
+        <v>154.11483999999999</v>
       </c>
       <c r="D2" s="18">
-        <v>47.772624999999998</v>
+        <v>43.642200000000003</v>
       </c>
       <c r="E2" s="18">
-        <v>77.720849999999999</v>
+        <v>77.350173999999996</v>
       </c>
       <c r="F2" s="18">
-        <v>8.0260960000000008</v>
+        <v>7.9939245999999997</v>
       </c>
       <c r="K2" s="18">
-        <v>704.45479999999998</v>
+        <v>712.71559999999999</v>
       </c>
       <c r="M2" s="18">
         <v>100</v>
@@ -996,19 +1043,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="18">
-        <v>132.59293</v>
+        <v>135.26382000000001</v>
       </c>
       <c r="D3" s="18">
-        <v>41.17015</v>
+        <v>43.943947000000001</v>
       </c>
       <c r="E3" s="18">
-        <v>77.811676000000006</v>
+        <v>78.896910000000005</v>
       </c>
       <c r="F3" s="18">
-        <v>7.9754149999999999</v>
+        <v>7.9605655999999998</v>
       </c>
       <c r="K3" s="18">
-        <v>717.65967000000001</v>
+        <v>712.11210000000005</v>
       </c>
       <c r="M3" s="18">
         <v>100</v>
@@ -1022,19 +1069,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="18">
-        <v>126.65949999999999</v>
+        <v>137.17693</v>
       </c>
       <c r="D4" s="18">
-        <v>36.895350000000001</v>
+        <v>41.257137</v>
       </c>
       <c r="E4" s="18">
-        <v>87.052480000000003</v>
+        <v>82.116669999999999</v>
       </c>
       <c r="F4" s="18">
-        <v>9.0067830000000004</v>
+        <v>9.0071060000000003</v>
       </c>
       <c r="K4" s="18">
-        <v>743.79534999999998</v>
+        <v>732.78549999999996</v>
       </c>
       <c r="M4" s="18">
         <v>100</v>
@@ -1048,19 +1095,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="18">
-        <v>152.86093</v>
+        <v>151.01679999999999</v>
       </c>
       <c r="D5" s="18">
-        <v>49.037599999999998</v>
+        <v>45.442585000000001</v>
       </c>
       <c r="E5" s="18">
-        <v>80.05838</v>
+        <v>81.772620000000003</v>
       </c>
       <c r="F5" s="18">
-        <v>8.040832</v>
+        <v>8.0394570000000005</v>
       </c>
       <c r="K5" s="18">
-        <v>701.9248</v>
+        <v>709.11479999999995</v>
       </c>
       <c r="M5" s="18">
         <v>100</v>
@@ -1074,19 +1121,19 @@
         <v>4</v>
       </c>
       <c r="C6" s="18">
-        <v>120.15527</v>
+        <v>144.70716999999999</v>
       </c>
       <c r="D6" s="18">
-        <v>41.633384999999997</v>
+        <v>41.703795999999997</v>
       </c>
       <c r="E6" s="18">
-        <v>81.704610000000002</v>
+        <v>72.932659999999998</v>
       </c>
       <c r="F6" s="18">
-        <v>8.9980650000000004</v>
+        <v>7.9775714999999998</v>
       </c>
       <c r="K6" s="18">
-        <v>735.88696000000004</v>
+        <v>716.5924</v>
       </c>
       <c r="M6" s="18">
         <v>100</v>
@@ -1100,19 +1147,19 @@
         <v>5</v>
       </c>
       <c r="C7" s="18">
-        <v>138.74258</v>
+        <v>132.75253000000001</v>
       </c>
       <c r="D7" s="18">
-        <v>45.983739999999997</v>
+        <v>56.748710000000003</v>
       </c>
       <c r="E7" s="18">
-        <v>74.826096000000007</v>
+        <v>74.382739999999998</v>
       </c>
       <c r="F7" s="18">
-        <v>8.0412245000000002</v>
+        <v>8.0051640000000006</v>
       </c>
       <c r="K7" s="18">
-        <v>708.03252999999995</v>
+        <v>686.50256000000002</v>
       </c>
       <c r="M7" s="18">
         <v>100</v>
@@ -1126,19 +1173,19 @@
         <v>6</v>
       </c>
       <c r="C8" s="18">
-        <v>130.17908</v>
+        <v>110.82988</v>
       </c>
       <c r="D8" s="18">
-        <v>47.343600000000002</v>
+        <v>40.969242000000001</v>
       </c>
       <c r="E8" s="18">
-        <v>78.907079999999993</v>
+        <v>79.494529999999997</v>
       </c>
       <c r="F8" s="18">
-        <v>7.991104</v>
+        <v>8.0053920000000005</v>
       </c>
       <c r="K8" s="18">
-        <v>705.31280000000004</v>
+        <v>718.06150000000002</v>
       </c>
       <c r="M8" s="18">
         <v>100</v>
@@ -1152,19 +1199,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="18">
-        <v>114.93615</v>
+        <v>128.91692</v>
       </c>
       <c r="D9" s="18">
-        <v>37.872272000000002</v>
+        <v>49.261710000000001</v>
       </c>
       <c r="E9" s="18">
-        <v>83.513959999999997</v>
+        <v>78.051349999999999</v>
       </c>
       <c r="F9" s="18">
-        <v>9.0284479999999991</v>
+        <v>7.973954</v>
       </c>
       <c r="K9" s="18">
-        <v>741.00019999999995</v>
+        <v>701.47655999999995</v>
       </c>
       <c r="M9" s="18">
         <v>100</v>
@@ -1178,19 +1225,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="18">
-        <v>155.03648000000001</v>
+        <v>158.06413000000001</v>
       </c>
       <c r="D10" s="18">
-        <v>45.076782000000001</v>
+        <v>45.962643</v>
       </c>
       <c r="E10" s="18">
-        <v>81.160610000000005</v>
+        <v>80.426699999999997</v>
       </c>
       <c r="F10" s="18">
-        <v>7.9671282999999997</v>
+        <v>7.9709085999999996</v>
       </c>
       <c r="K10" s="18">
-        <v>709.84644000000003</v>
+        <v>708.07470000000001</v>
       </c>
       <c r="M10" s="18">
         <v>100</v>
@@ -1204,19 +1251,19 @@
         <v>9</v>
       </c>
       <c r="C11" s="18">
-        <v>99.267880000000005</v>
+        <v>132.39804000000001</v>
       </c>
       <c r="D11" s="18">
-        <v>41.224505999999998</v>
+        <v>37.272219999999997</v>
       </c>
       <c r="E11" s="18">
-        <v>84.812706000000006</v>
+        <v>72.816810000000004</v>
       </c>
       <c r="F11" s="18">
-        <v>8.9901704999999996</v>
+        <v>7.9794025</v>
       </c>
       <c r="K11" s="18">
-        <v>735.42240000000004</v>
+        <v>725.45556999999997</v>
       </c>
       <c r="M11" s="18">
         <v>100</v>
@@ -1230,19 +1277,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="18">
-        <v>127.237076</v>
+        <v>127.907104</v>
       </c>
       <c r="D12" s="18">
-        <v>36.209316000000001</v>
+        <v>54.351944000000003</v>
       </c>
       <c r="E12" s="18">
-        <v>76.456670000000003</v>
+        <v>77.109790000000004</v>
       </c>
       <c r="F12" s="18">
-        <v>8.0060490000000009</v>
+        <v>7.9946603999999999</v>
       </c>
       <c r="K12" s="18">
-        <v>727.58136000000002</v>
+        <v>691.29614000000004</v>
       </c>
       <c r="M12" s="18">
         <v>100</v>
@@ -1256,19 +1303,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="18">
-        <v>116.92</v>
+        <v>138.47273000000001</v>
       </c>
       <c r="D13" s="18">
-        <v>48.604709999999997</v>
+        <v>38.905678000000002</v>
       </c>
       <c r="E13" s="18">
-        <v>75.416759999999996</v>
+        <v>74.381140000000002</v>
       </c>
       <c r="F13" s="18">
-        <v>8.0238990000000001</v>
+        <v>8.0133840000000003</v>
       </c>
       <c r="K13" s="18">
-        <v>702.79060000000004</v>
+        <v>722.18866000000003</v>
       </c>
       <c r="M13" s="18">
         <v>100</v>
@@ -1282,19 +1329,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="18">
-        <v>126.52513</v>
+        <v>104.50162</v>
       </c>
       <c r="D14" s="18">
-        <v>46.915897000000001</v>
+        <v>36.205199999999998</v>
       </c>
       <c r="E14" s="18">
-        <v>74.839619999999996</v>
+        <v>87.193984999999998</v>
       </c>
       <c r="F14" s="18">
-        <v>8.0303970000000007</v>
+        <v>8.9990260000000006</v>
       </c>
       <c r="K14" s="18">
-        <v>706.16819999999996</v>
+        <v>743.09960000000001</v>
       </c>
       <c r="M14" s="18">
         <v>100</v>
@@ -1308,19 +1355,19 @@
         <v>13</v>
       </c>
       <c r="C15" s="18">
-        <v>135.3777</v>
+        <v>137.46878000000001</v>
       </c>
       <c r="D15" s="18">
-        <v>45.41131</v>
+        <v>46.051822999999999</v>
       </c>
       <c r="E15" s="18">
-        <v>73.949370000000002</v>
+        <v>79.234430000000003</v>
       </c>
       <c r="F15" s="18">
-        <v>8.0001479999999994</v>
+        <v>8.0342040000000008</v>
       </c>
       <c r="K15" s="18">
-        <v>709.17737</v>
+        <v>707.89635999999996</v>
       </c>
       <c r="M15" s="18">
         <v>100</v>
@@ -1334,19 +1381,19 @@
         <v>14</v>
       </c>
       <c r="C16" s="18">
-        <v>136.34392</v>
+        <v>109.3082</v>
       </c>
       <c r="D16" s="18">
-        <v>53.264279999999999</v>
+        <v>45.919727000000002</v>
       </c>
       <c r="E16" s="18">
-        <v>77.564170000000004</v>
+        <v>76.000786000000005</v>
       </c>
       <c r="F16" s="18">
-        <v>7.9981154999999999</v>
+        <v>8.0064270000000004</v>
       </c>
       <c r="K16" s="18">
-        <v>693.47144000000003</v>
+        <v>708.16049999999996</v>
       </c>
       <c r="M16" s="18">
         <v>100</v>
@@ -1360,19 +1407,19 @@
         <v>15</v>
       </c>
       <c r="C17" s="18">
-        <v>142.10538</v>
+        <v>118.0057</v>
       </c>
       <c r="D17" s="18">
-        <v>50.192450000000001</v>
+        <v>51.396422999999999</v>
       </c>
       <c r="E17" s="18">
-        <v>76.920479999999998</v>
+        <v>78.807919999999996</v>
       </c>
       <c r="F17" s="18">
-        <v>8.0215460000000007</v>
+        <v>8.0014420000000008</v>
       </c>
       <c r="K17" s="18">
-        <v>699.61509999999998</v>
+        <v>697.20714999999996</v>
       </c>
       <c r="M17" s="18">
         <v>100</v>
@@ -1386,19 +1433,19 @@
         <v>16</v>
       </c>
       <c r="C18" s="18">
-        <v>124.67924499999999</v>
+        <v>106.7206</v>
       </c>
       <c r="D18" s="18">
-        <v>42.147235999999999</v>
+        <v>46.489649999999997</v>
       </c>
       <c r="E18" s="18">
-        <v>78.430695</v>
+        <v>76.581630000000004</v>
       </c>
       <c r="F18" s="18">
-        <v>7.9957190000000002</v>
+        <v>8.0111950000000007</v>
       </c>
       <c r="K18" s="18">
-        <v>715.70550000000003</v>
+        <v>707.02070000000003</v>
       </c>
       <c r="M18" s="18">
         <v>100</v>
@@ -1412,19 +1459,19 @@
         <v>17</v>
       </c>
       <c r="C19" s="18">
-        <v>124.45135500000001</v>
+        <v>123.3125</v>
       </c>
       <c r="D19" s="18">
-        <v>51.573784000000003</v>
+        <v>42.297170000000001</v>
       </c>
       <c r="E19" s="18">
-        <v>75.168304000000006</v>
+        <v>74.414444000000003</v>
       </c>
       <c r="F19" s="18">
-        <v>7.9948759999999996</v>
+        <v>7.9728760000000003</v>
       </c>
       <c r="K19" s="18">
-        <v>696.85239999999999</v>
+        <v>715.40563999999995</v>
       </c>
       <c r="M19" s="18">
         <v>100</v>
@@ -1438,19 +1485,19 @@
         <v>18</v>
       </c>
       <c r="C20" s="18">
-        <v>136.01288</v>
+        <v>148.03322</v>
       </c>
       <c r="D20" s="18">
-        <v>40.407829999999997</v>
+        <v>46.769317999999998</v>
       </c>
       <c r="E20" s="18">
-        <v>78.355609999999999</v>
+        <v>78.34966</v>
       </c>
       <c r="F20" s="18">
-        <v>8.0193100000000008</v>
+        <v>7.9754069999999997</v>
       </c>
       <c r="K20" s="18">
-        <v>719.18430000000001</v>
+        <v>706.46136000000001</v>
       </c>
       <c r="M20" s="18">
         <v>100</v>
@@ -1464,19 +1511,19 @@
         <v>19</v>
       </c>
       <c r="C21" s="18">
-        <v>150.62102999999999</v>
+        <v>157.95724000000001</v>
       </c>
       <c r="D21" s="18">
-        <v>53.514029999999998</v>
+        <v>44.241591999999997</v>
       </c>
       <c r="E21" s="18">
-        <v>77.490160000000003</v>
+        <v>88.046700000000001</v>
       </c>
       <c r="F21" s="18">
-        <v>7.9807433999999997</v>
+        <v>8.9932719999999993</v>
       </c>
       <c r="K21" s="18">
-        <v>692.97190000000001</v>
+        <v>729.90575999999999</v>
       </c>
       <c r="M21" s="18">
         <v>100</v>
@@ -1490,19 +1537,19 @@
         <v>20</v>
       </c>
       <c r="C22" s="18">
-        <v>114.34936999999999</v>
+        <v>116.77434</v>
       </c>
       <c r="D22" s="18">
-        <v>36.828163000000004</v>
+        <v>40.190365</v>
       </c>
       <c r="E22" s="18">
-        <v>73.849770000000007</v>
+        <v>84.865660000000005</v>
       </c>
       <c r="F22" s="18">
-        <v>8.0200549999999993</v>
+        <v>8.9564409999999999</v>
       </c>
       <c r="K22" s="18">
-        <v>726.34370000000001</v>
+        <v>742.63214000000005</v>
       </c>
       <c r="M22" s="18">
         <v>100</v>
@@ -1516,19 +1563,19 @@
         <v>21</v>
       </c>
       <c r="C23" s="18">
-        <v>155.82272</v>
+        <v>137.20638</v>
       </c>
       <c r="D23" s="18">
-        <v>47.975270000000002</v>
+        <v>38.30829</v>
       </c>
       <c r="E23" s="18">
-        <v>79.897329999999997</v>
+        <v>77.294240000000002</v>
       </c>
       <c r="F23" s="18">
-        <v>7.9940566999999998</v>
+        <v>7.9849953999999999</v>
       </c>
       <c r="K23" s="18">
-        <v>704.04944</v>
+        <v>723.38340000000005</v>
       </c>
       <c r="M23" s="18">
         <v>100</v>
@@ -1542,19 +1589,19 @@
         <v>22</v>
       </c>
       <c r="C24" s="18">
-        <v>130.67496</v>
+        <v>126.05419999999999</v>
       </c>
       <c r="D24" s="18">
-        <v>48.043956999999999</v>
+        <v>33.582096</v>
       </c>
       <c r="E24" s="18">
-        <v>90.620636000000005</v>
+        <v>79.694046</v>
       </c>
       <c r="F24" s="18">
-        <v>8.9831889999999994</v>
+        <v>7.9771131999999998</v>
       </c>
       <c r="K24" s="18">
-        <v>718.95012999999994</v>
+        <v>732.83579999999995</v>
       </c>
       <c r="M24" s="18">
         <v>100</v>
@@ -1568,19 +1615,19 @@
         <v>23</v>
       </c>
       <c r="C25" s="18">
-        <v>135.60120000000001</v>
+        <v>107.9663</v>
       </c>
       <c r="D25" s="18">
-        <v>56.176346000000002</v>
+        <v>40.060096999999999</v>
       </c>
       <c r="E25" s="18">
-        <v>87.862114000000005</v>
+        <v>78.356449999999995</v>
       </c>
       <c r="F25" s="18">
-        <v>8.9909350000000003</v>
+        <v>7.9946275</v>
       </c>
       <c r="K25" s="18">
-        <v>704.57910000000004</v>
+        <v>719.87980000000005</v>
       </c>
       <c r="M25" s="18">
         <v>100</v>
@@ -1594,19 +1641,19 @@
         <v>24</v>
       </c>
       <c r="C26" s="18">
-        <v>154.05969999999999</v>
+        <v>129.80348000000001</v>
       </c>
       <c r="D26" s="18">
-        <v>58.840224999999997</v>
+        <v>50.977623000000001</v>
       </c>
       <c r="E26" s="18">
-        <v>74.785330000000002</v>
+        <v>77.684179999999998</v>
       </c>
       <c r="F26" s="18">
-        <v>8.0165740000000003</v>
+        <v>7.9597309999999997</v>
       </c>
       <c r="K26" s="18">
-        <v>682.31960000000004</v>
+        <v>698.04474000000005</v>
       </c>
       <c r="M26" s="18">
         <v>100</v>
@@ -1620,19 +1667,19 @@
         <v>25</v>
       </c>
       <c r="C27" s="18">
-        <v>126.3612</v>
+        <v>118.34923000000001</v>
       </c>
       <c r="D27" s="18">
-        <v>54.745185999999997</v>
+        <v>37.083595000000003</v>
       </c>
       <c r="E27" s="18">
-        <v>89.269135000000006</v>
+        <v>78.876390000000001</v>
       </c>
       <c r="F27" s="18">
-        <v>8.9734079999999992</v>
+        <v>7.9929503999999998</v>
       </c>
       <c r="K27" s="18">
-        <v>708.1825</v>
+        <v>725.83280000000002</v>
       </c>
       <c r="M27" s="18">
         <v>100</v>
@@ -1646,19 +1693,19 @@
         <v>26</v>
       </c>
       <c r="C28" s="18">
-        <v>122.05159</v>
+        <v>123.50893000000001</v>
       </c>
       <c r="D28" s="18">
-        <v>43.778056999999997</v>
+        <v>52.09854</v>
       </c>
       <c r="E28" s="18">
-        <v>71.666954000000004</v>
+        <v>79.297966000000002</v>
       </c>
       <c r="F28" s="18">
-        <v>7.9749699999999999</v>
+        <v>8.0076900000000002</v>
       </c>
       <c r="K28" s="18">
-        <v>712.44389999999999</v>
+        <v>695.80290000000002</v>
       </c>
       <c r="M28" s="18">
         <v>100</v>
@@ -1672,19 +1719,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="18">
-        <v>116.29452999999999</v>
+        <v>110.214905</v>
       </c>
       <c r="D29" s="18">
-        <v>44.946278</v>
+        <v>42.074719999999999</v>
       </c>
       <c r="E29" s="18">
-        <v>78.943380000000005</v>
+        <v>72.879279999999994</v>
       </c>
       <c r="F29" s="18">
-        <v>8.0225249999999999</v>
+        <v>8.0110089999999996</v>
       </c>
       <c r="K29" s="18">
-        <v>710.10739999999998</v>
+        <v>715.85059999999999</v>
       </c>
       <c r="M29" s="18">
         <v>100</v>
@@ -1698,19 +1745,19 @@
         <v>28</v>
       </c>
       <c r="C30" s="18">
-        <v>137.18974</v>
+        <v>127.34936999999999</v>
       </c>
       <c r="D30" s="18">
-        <v>44.740887000000001</v>
+        <v>42.757840000000002</v>
       </c>
       <c r="E30" s="18">
-        <v>85.044899999999998</v>
+        <v>76.374309999999994</v>
       </c>
       <c r="F30" s="18">
-        <v>9.0316550000000007</v>
+        <v>7.9898442999999997</v>
       </c>
       <c r="K30" s="18">
-        <v>726.41125</v>
+        <v>714.48429999999996</v>
       </c>
       <c r="M30" s="18">
         <v>100</v>
@@ -1724,19 +1771,19 @@
         <v>29</v>
       </c>
       <c r="C31" s="18">
-        <v>118.84717000000001</v>
+        <v>158.68983</v>
       </c>
       <c r="D31" s="18">
-        <v>36.653163999999997</v>
+        <v>56.674239999999998</v>
       </c>
       <c r="E31" s="18">
-        <v>77.294785000000005</v>
+        <v>77.96163</v>
       </c>
       <c r="F31" s="18">
-        <v>7.969061</v>
+        <v>7.9881487</v>
       </c>
       <c r="K31" s="18">
-        <v>726.69366000000002</v>
+        <v>686.65150000000006</v>
       </c>
       <c r="M31" s="18">
         <v>100</v>
@@ -1750,19 +1797,19 @@
         <v>30</v>
       </c>
       <c r="C32" s="18">
-        <v>128.52634</v>
+        <v>120.88579</v>
       </c>
       <c r="D32" s="18">
-        <v>45.677093999999997</v>
+        <v>47.304366999999999</v>
       </c>
       <c r="E32" s="18">
-        <v>79.626784999999998</v>
+        <v>77.741560000000007</v>
       </c>
       <c r="F32" s="18">
-        <v>8.0070080000000008</v>
+        <v>8.004702</v>
       </c>
       <c r="K32" s="18">
-        <v>708.64580000000001</v>
+        <v>705.39124000000004</v>
       </c>
       <c r="M32" s="18">
         <v>100</v>
@@ -1776,19 +1823,19 @@
         <v>31</v>
       </c>
       <c r="C33" s="18">
-        <v>107.35567</v>
+        <v>157.32159999999999</v>
       </c>
       <c r="D33" s="18">
-        <v>41.586799999999997</v>
+        <v>50.601570000000002</v>
       </c>
       <c r="E33" s="18">
-        <v>73.560609999999997</v>
+        <v>98.034019999999998</v>
       </c>
       <c r="F33" s="18">
-        <v>7.9412409999999998</v>
+        <v>9.9771190000000001</v>
       </c>
       <c r="K33" s="18">
-        <v>716.82640000000004</v>
+        <v>737.84230000000002</v>
       </c>
       <c r="M33" s="18">
         <v>100</v>
@@ -1802,19 +1849,19 @@
         <v>32</v>
       </c>
       <c r="C34" s="18">
-        <v>114.585594</v>
+        <v>131.07782</v>
       </c>
       <c r="D34" s="18">
-        <v>46.633102000000001</v>
+        <v>52.459569999999999</v>
       </c>
       <c r="E34" s="18">
-        <v>72.391689999999997</v>
+        <v>78.465639999999993</v>
       </c>
       <c r="F34" s="18">
-        <v>7.9894604999999999</v>
+        <v>8.0131580000000007</v>
       </c>
       <c r="K34" s="18">
-        <v>706.73375999999996</v>
+        <v>695.08090000000004</v>
       </c>
       <c r="M34" s="18">
         <v>100</v>
@@ -1828,19 +1875,19 @@
         <v>33</v>
       </c>
       <c r="C35" s="18">
-        <v>135.43933000000001</v>
+        <v>149.68243000000001</v>
       </c>
       <c r="D35" s="18">
-        <v>43.677950000000003</v>
+        <v>49.835616999999999</v>
       </c>
       <c r="E35" s="18">
-        <v>80.19162</v>
+        <v>81.245609999999999</v>
       </c>
       <c r="F35" s="18">
-        <v>8.0231290000000008</v>
+        <v>8.0227529999999998</v>
       </c>
       <c r="K35" s="18">
-        <v>712.64409999999998</v>
+        <v>700.32874000000004</v>
       </c>
       <c r="M35" s="18">
         <v>100</v>
@@ -1854,21 +1901,203 @@
         <v>34</v>
       </c>
       <c r="C36" s="18">
-        <v>111.054695</v>
+        <v>124.91701999999999</v>
       </c>
       <c r="D36" s="18">
-        <v>41.543182000000002</v>
+        <v>49.243766999999998</v>
       </c>
       <c r="E36" s="18">
-        <v>87.356920000000002</v>
+        <v>75.406525000000002</v>
       </c>
       <c r="F36" s="18">
-        <v>9.0094480000000008</v>
+        <v>7.9821463000000001</v>
       </c>
       <c r="K36" s="18">
-        <v>732.12463000000002</v>
+        <v>701.51244999999994</v>
       </c>
       <c r="M36" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9">
+        <v>35</v>
+      </c>
+      <c r="C37" s="18">
+        <v>121.76888</v>
+      </c>
+      <c r="D37" s="18">
+        <v>49.243766999999998</v>
+      </c>
+      <c r="E37" s="18">
+        <v>75.722880000000004</v>
+      </c>
+      <c r="F37" s="18">
+        <v>7.9866609999999998</v>
+      </c>
+      <c r="K37" s="18">
+        <v>701.51244999999994</v>
+      </c>
+      <c r="M37" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="9">
+        <v>36</v>
+      </c>
+      <c r="C38" s="18">
+        <v>115.950165</v>
+      </c>
+      <c r="D38" s="18">
+        <v>49.598300000000002</v>
+      </c>
+      <c r="E38" s="18">
+        <v>89.644800000000004</v>
+      </c>
+      <c r="F38" s="18">
+        <v>8.9962160000000004</v>
+      </c>
+      <c r="K38" s="18">
+        <v>717.3279</v>
+      </c>
+      <c r="M38" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>2</v>
+      </c>
+      <c r="B39" s="9">
+        <v>37</v>
+      </c>
+      <c r="C39" s="18">
+        <v>117.660645</v>
+      </c>
+      <c r="D39" s="18">
+        <v>51.396422999999999</v>
+      </c>
+      <c r="E39" s="18">
+        <v>78.787019999999998</v>
+      </c>
+      <c r="F39" s="18">
+        <v>7.9948335000000004</v>
+      </c>
+      <c r="K39" s="18">
+        <v>697.20714999999996</v>
+      </c>
+      <c r="M39" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="9">
+        <v>38</v>
+      </c>
+      <c r="C40" s="18">
+        <v>124.22832</v>
+      </c>
+      <c r="D40" s="18">
+        <v>51.396422999999999</v>
+      </c>
+      <c r="E40" s="18">
+        <v>78.606589999999997</v>
+      </c>
+      <c r="F40" s="18">
+        <v>8.0082369999999994</v>
+      </c>
+      <c r="K40" s="18">
+        <v>697.20714999999996</v>
+      </c>
+      <c r="M40" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>2</v>
+      </c>
+      <c r="B41" s="9">
+        <v>39</v>
+      </c>
+      <c r="C41" s="18">
+        <v>128.18270000000001</v>
+      </c>
+      <c r="D41" s="18">
+        <v>51.592776999999998</v>
+      </c>
+      <c r="E41" s="18">
+        <v>90.281499999999994</v>
+      </c>
+      <c r="F41" s="18">
+        <v>9.0038009999999993</v>
+      </c>
+      <c r="K41" s="18">
+        <v>712.33527000000004</v>
+      </c>
+      <c r="M41" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9">
+        <v>40</v>
+      </c>
+      <c r="C42" s="18">
+        <v>123.441574</v>
+      </c>
+      <c r="D42" s="18">
+        <v>56.568497000000001</v>
+      </c>
+      <c r="E42" s="18">
+        <v>90.408844000000002</v>
+      </c>
+      <c r="F42" s="18">
+        <v>9.9916689999999999</v>
+      </c>
+      <c r="K42" s="18">
+        <v>719.76733000000002</v>
+      </c>
+      <c r="M42" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>2</v>
+      </c>
+      <c r="B43" s="9">
+        <v>41</v>
+      </c>
+      <c r="C43" s="18">
+        <v>115.41699</v>
+      </c>
+      <c r="D43" s="18">
+        <v>50.897820000000003</v>
+      </c>
+      <c r="E43" s="18">
+        <v>78.195080000000004</v>
+      </c>
+      <c r="F43" s="18">
+        <v>8.0004829999999991</v>
+      </c>
+      <c r="K43" s="18">
+        <v>698.20434999999998</v>
+      </c>
+      <c r="M43" s="18">
         <v>100</v>
       </c>
     </row>
@@ -1879,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" activeCellId="1" sqref="F1:F1048576 H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,38 +2169,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15">
-        <v>129.06763000000001</v>
-      </c>
-      <c r="C2" s="15">
-        <v>45.545623999999997</v>
-      </c>
-      <c r="D2" s="15">
-        <v>79.272049999999993</v>
-      </c>
-      <c r="E2" s="15">
-        <v>8.2595080000000003</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="15">
-        <v>0</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15">
-        <v>0</v>
-      </c>
-      <c r="J2" s="15">
-        <v>713.25463999999999</v>
-      </c>
-      <c r="K2" s="15">
-        <v>0</v>
-      </c>
-      <c r="L2" s="15">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28">
+        <v>131.33516</v>
+      </c>
+      <c r="C2" s="28">
+        <v>45.202427</v>
+      </c>
+      <c r="D2" s="28">
+        <v>78.929680000000005</v>
+      </c>
+      <c r="E2" s="28">
+        <v>8.1650790000000004</v>
+      </c>
+      <c r="F2" s="28">
+        <v>0</v>
+      </c>
+      <c r="G2" s="28">
+        <v>0</v>
+      </c>
+      <c r="H2" s="28">
+        <v>0</v>
+      </c>
+      <c r="I2" s="28">
+        <v>0</v>
+      </c>
+      <c r="J2" s="28">
+        <v>712.77373999999998</v>
+      </c>
+      <c r="K2" s="28">
+        <v>0</v>
+      </c>
+      <c r="L2" s="28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27">
+        <v>120.9499</v>
+      </c>
+      <c r="C3" s="27">
+        <v>51.527718</v>
+      </c>
+      <c r="D3" s="27">
+        <v>83.092389999999995</v>
+      </c>
+      <c r="E3" s="27">
+        <v>8.5688420000000001</v>
+      </c>
+      <c r="F3" s="27">
+        <v>0</v>
+      </c>
+      <c r="G3" s="27">
+        <v>0</v>
+      </c>
+      <c r="H3" s="27">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27">
+        <v>0</v>
+      </c>
+      <c r="J3" s="27">
+        <v>706.22310000000004</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0</v>
+      </c>
+      <c r="L3" s="29">
         <v>100</v>
       </c>
     </row>
@@ -1982,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,7 +2264,7 @@
     <col min="3" max="4" width="11" style="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2018,29 +2287,987 @@
         <v>27</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23">
+        <v>53</v>
+      </c>
+      <c r="D2" s="23">
+        <v>-17</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0</v>
+      </c>
+      <c r="F2" s="19">
+        <v>10.007555</v>
+      </c>
+      <c r="G2" s="19">
+        <v>100.00436999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24">
+        <v>-27</v>
+      </c>
+      <c r="D3" s="24">
+        <v>49</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0</v>
+      </c>
+      <c r="F3" s="18">
+        <v>10.013244</v>
+      </c>
+      <c r="G3" s="18">
+        <v>99.992009999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24">
+        <v>48</v>
+      </c>
+      <c r="D4" s="24">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="18">
+        <v>9.9980440000000002</v>
+      </c>
+      <c r="G4" s="18">
+        <v>100.00006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="24">
+        <v>48</v>
+      </c>
+      <c r="D5" s="24">
+        <v>29</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="18">
+        <v>9.9964510000000004</v>
+      </c>
+      <c r="G5" s="18">
+        <v>99.990110000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="24">
+        <v>6</v>
+      </c>
+      <c r="D6" s="24">
+        <v>-55</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="18">
+        <v>10.001097</v>
+      </c>
+      <c r="G6" s="18">
+        <v>99.996409999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="24">
+        <v>42</v>
+      </c>
+      <c r="D7" s="24">
+        <v>-36</v>
+      </c>
+      <c r="E7" s="24">
+        <v>2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>9.9898740000000004</v>
+      </c>
+      <c r="G7" s="18">
+        <v>100.01863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="24">
+        <v>55</v>
+      </c>
+      <c r="D8" s="24">
+        <v>8</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>10.006026</v>
+      </c>
+      <c r="G8" s="18">
+        <v>99.995804000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="24">
+        <v>49</v>
+      </c>
+      <c r="D9" s="24">
+        <v>-27</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <v>10.000956</v>
+      </c>
+      <c r="G9" s="18">
+        <v>100.00378000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+      <c r="C10" s="24">
+        <v>-19</v>
+      </c>
+      <c r="D10" s="24">
+        <v>52</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18">
+        <v>9.9986300000000004</v>
+      </c>
+      <c r="G10" s="18">
+        <v>99.994669999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+      <c r="C11" s="24">
+        <v>51</v>
+      </c>
+      <c r="D11" s="24">
+        <v>23</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18">
+        <v>9.9918270000000007</v>
+      </c>
+      <c r="G11" s="18">
+        <v>100.01507599999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="24">
+        <v>-22</v>
+      </c>
+      <c r="D12" s="24">
+        <v>-51</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18">
+        <v>10.004405999999999</v>
+      </c>
+      <c r="G12" s="18">
+        <v>100.00838</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="24">
+        <v>50</v>
+      </c>
+      <c r="D13" s="24">
+        <v>-24</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18">
+        <v>10.00536</v>
+      </c>
+      <c r="G13" s="18">
+        <v>100.00604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="24">
+        <v>56</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18">
+        <v>10.010899</v>
+      </c>
+      <c r="G14" s="18">
+        <v>99.998474000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="24">
+        <v>-44</v>
+      </c>
+      <c r="D15" s="24">
+        <v>-34</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="18">
+        <v>9.9993870000000005</v>
+      </c>
+      <c r="G15" s="18">
+        <v>100.00391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+      <c r="C16" s="24">
+        <v>52</v>
+      </c>
+      <c r="D16" s="24">
+        <v>19</v>
+      </c>
+      <c r="E16" s="24">
+        <v>0</v>
+      </c>
+      <c r="F16" s="18">
+        <v>10.004600999999999</v>
+      </c>
+      <c r="G16" s="18">
+        <v>99.998750000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+      <c r="C17" s="24">
+        <v>41</v>
+      </c>
+      <c r="D17" s="24">
+        <v>37</v>
+      </c>
+      <c r="E17" s="24">
+        <v>8</v>
+      </c>
+      <c r="F17" s="18">
+        <v>10.006848</v>
+      </c>
+      <c r="G17" s="18">
+        <v>100.00333999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+      <c r="C18" s="24">
+        <v>55</v>
+      </c>
+      <c r="D18" s="24">
+        <v>9</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>9.9989329999999992</v>
+      </c>
+      <c r="G18" s="18">
+        <v>100.00233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9">
+        <v>17</v>
+      </c>
+      <c r="C19" s="24">
+        <v>-10</v>
+      </c>
+      <c r="D19" s="24">
+        <v>-55</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="F19" s="18">
+        <v>10.004882</v>
+      </c>
+      <c r="G19" s="18">
+        <v>99.992270000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9">
+        <v>18</v>
+      </c>
+      <c r="C20" s="24">
+        <v>17</v>
+      </c>
+      <c r="D20" s="24">
+        <v>-53</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+      <c r="F20" s="18">
+        <v>9.9934519999999996</v>
+      </c>
+      <c r="G20" s="18">
+        <v>99.995949999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9">
+        <v>19</v>
+      </c>
+      <c r="C21" s="24">
+        <v>-36</v>
+      </c>
+      <c r="D21" s="24">
+        <v>42</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0</v>
+      </c>
+      <c r="F21" s="18">
+        <v>10.000246000000001</v>
+      </c>
+      <c r="G21" s="18">
+        <v>100.02552</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="9">
+        <v>20</v>
+      </c>
+      <c r="C22" s="24">
+        <v>43</v>
+      </c>
+      <c r="D22" s="24">
+        <v>36</v>
+      </c>
+      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+      <c r="F22" s="18">
+        <v>10.000299</v>
+      </c>
+      <c r="G22" s="18">
+        <v>100.007065</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="9">
+        <v>21</v>
+      </c>
+      <c r="C23" s="24">
+        <v>54</v>
+      </c>
+      <c r="D23" s="24">
+        <v>12</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0</v>
+      </c>
+      <c r="F23" s="18">
+        <v>9.9920770000000001</v>
+      </c>
+      <c r="G23" s="18">
+        <v>99.996970000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9">
+        <v>22</v>
+      </c>
+      <c r="C24" s="24">
+        <v>31</v>
+      </c>
+      <c r="D24" s="24">
+        <v>-46</v>
+      </c>
+      <c r="E24" s="24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="18">
+        <v>9.9998319999999996</v>
+      </c>
+      <c r="G24" s="18">
+        <v>99.999274999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="9">
+        <v>23</v>
+      </c>
+      <c r="C25" s="24">
+        <v>-28</v>
+      </c>
+      <c r="D25" s="24">
+        <v>-48</v>
+      </c>
+      <c r="E25" s="24">
+        <v>0</v>
+      </c>
+      <c r="F25" s="18">
+        <v>10.002188</v>
+      </c>
+      <c r="G25" s="18">
+        <v>99.994254999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="9">
+        <v>24</v>
+      </c>
+      <c r="C26" s="24">
+        <v>-56</v>
+      </c>
+      <c r="D26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="24">
+        <v>0</v>
+      </c>
+      <c r="F26" s="18">
+        <v>9.9955359999999995</v>
+      </c>
+      <c r="G26" s="18">
+        <v>100.01031</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
+        <v>25</v>
+      </c>
+      <c r="C27" s="24">
+        <v>12</v>
+      </c>
+      <c r="D27" s="24">
+        <v>-54</v>
+      </c>
+      <c r="E27" s="24">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18">
+        <v>10.001887</v>
+      </c>
+      <c r="G27" s="18">
+        <v>100.00317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="9">
+        <v>26</v>
+      </c>
+      <c r="C28" s="24">
+        <v>55</v>
+      </c>
+      <c r="D28" s="24">
+        <v>8</v>
+      </c>
+      <c r="E28" s="24">
+        <v>0</v>
+      </c>
+      <c r="F28" s="18">
+        <v>10.0003805</v>
+      </c>
+      <c r="G28" s="18">
+        <v>99.996729999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9">
+        <v>27</v>
+      </c>
+      <c r="C29" s="24">
+        <v>28</v>
+      </c>
+      <c r="D29" s="24">
+        <v>48</v>
+      </c>
+      <c r="E29" s="24">
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <v>10.004334999999999</v>
+      </c>
+      <c r="G29" s="18">
+        <v>100.0031</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="9">
+        <v>28</v>
+      </c>
+      <c r="C30" s="24">
+        <v>-43</v>
+      </c>
+      <c r="D30" s="24">
+        <v>-35</v>
+      </c>
+      <c r="E30" s="24">
+        <v>0</v>
+      </c>
+      <c r="F30" s="18">
+        <v>10.009658999999999</v>
+      </c>
+      <c r="G30" s="18">
+        <v>100.00282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="9">
+        <v>29</v>
+      </c>
+      <c r="C31" s="24">
+        <v>-30</v>
+      </c>
+      <c r="D31" s="24">
+        <v>-47</v>
+      </c>
+      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+      <c r="F31" s="18">
+        <v>9.9977230000000006</v>
+      </c>
+      <c r="G31" s="18">
+        <v>100.00118000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="9">
+        <v>30</v>
+      </c>
+      <c r="C32" s="24">
+        <v>5</v>
+      </c>
+      <c r="D32" s="24">
+        <v>-55</v>
+      </c>
+      <c r="E32" s="24">
+        <v>0</v>
+      </c>
+      <c r="F32" s="18">
+        <v>9.9956999999999994</v>
+      </c>
+      <c r="G32" s="18">
+        <v>99.995316000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="9">
+        <v>31</v>
+      </c>
+      <c r="C33" s="24">
+        <v>-54</v>
+      </c>
+      <c r="D33" s="24">
+        <v>13</v>
+      </c>
+      <c r="E33" s="24">
+        <v>0</v>
+      </c>
+      <c r="F33" s="18">
+        <v>10.000954</v>
+      </c>
+      <c r="G33" s="18">
+        <v>100.00565</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="9">
+        <v>32</v>
+      </c>
+      <c r="C34" s="24">
+        <v>10</v>
+      </c>
+      <c r="D34" s="24">
+        <v>55</v>
+      </c>
+      <c r="E34" s="24">
+        <v>0</v>
+      </c>
+      <c r="F34" s="18">
+        <v>9.9960249999999995</v>
+      </c>
+      <c r="G34" s="18">
+        <v>99.991110000000006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="9">
+        <v>33</v>
+      </c>
+      <c r="C35" s="24">
+        <v>-8</v>
+      </c>
+      <c r="D35" s="24">
+        <v>-55</v>
+      </c>
+      <c r="E35" s="24">
+        <v>0</v>
+      </c>
+      <c r="F35" s="18">
+        <v>9.9971069999999997</v>
+      </c>
+      <c r="G35" s="18">
+        <v>100.00614</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9">
+        <v>34</v>
+      </c>
+      <c r="C36" s="24">
+        <v>-34</v>
+      </c>
+      <c r="D36" s="24">
+        <v>-44</v>
+      </c>
+      <c r="E36" s="24">
+        <v>5</v>
+      </c>
+      <c r="F36" s="18">
+        <v>9.9992529999999995</v>
+      </c>
+      <c r="G36" s="18">
+        <v>100.00185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9">
+        <v>35</v>
+      </c>
+      <c r="C37" s="24">
+        <v>-22</v>
+      </c>
+      <c r="D37" s="24">
+        <v>-24</v>
+      </c>
+      <c r="E37" s="24">
+        <v>0</v>
+      </c>
+      <c r="F37" s="18">
+        <v>9.9980290000000007</v>
+      </c>
+      <c r="G37" s="18">
+        <v>99.979830000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="9">
+        <v>36</v>
+      </c>
+      <c r="C38" s="24">
+        <v>-19</v>
+      </c>
+      <c r="D38" s="24">
+        <v>-19</v>
+      </c>
+      <c r="E38" s="24">
+        <v>0</v>
+      </c>
+      <c r="F38" s="18">
+        <v>9.995298</v>
+      </c>
+      <c r="G38" s="18">
+        <v>99.984380000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>2</v>
+      </c>
+      <c r="B39" s="9">
+        <v>37</v>
+      </c>
+      <c r="C39" s="24">
+        <v>19</v>
+      </c>
+      <c r="D39" s="24">
+        <v>19</v>
+      </c>
+      <c r="E39" s="24">
+        <v>0</v>
+      </c>
+      <c r="F39" s="18">
+        <v>10.012199000000001</v>
+      </c>
+      <c r="G39" s="18">
+        <v>100.00342999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="9">
+        <v>38</v>
+      </c>
+      <c r="C40" s="24">
+        <v>22</v>
+      </c>
+      <c r="D40" s="24">
+        <v>23</v>
+      </c>
+      <c r="E40" s="24">
+        <v>0</v>
+      </c>
+      <c r="F40" s="18">
+        <v>10.011803</v>
+      </c>
+      <c r="G40" s="18">
+        <v>100.00424</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>2</v>
+      </c>
+      <c r="B41" s="9">
+        <v>39</v>
+      </c>
+      <c r="C41" s="24">
+        <v>21</v>
+      </c>
+      <c r="D41" s="24">
+        <v>15</v>
+      </c>
+      <c r="E41" s="24">
+        <v>0</v>
+      </c>
+      <c r="F41" s="18">
+        <v>10.013456</v>
+      </c>
+      <c r="G41" s="18">
+        <v>100.00694</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9">
+        <v>40</v>
+      </c>
+      <c r="C42" s="24">
+        <v>17</v>
+      </c>
+      <c r="D42" s="24">
+        <v>-15</v>
+      </c>
+      <c r="E42" s="24">
+        <v>0</v>
+      </c>
+      <c r="F42" s="18">
+        <v>9.9902949999999997</v>
+      </c>
+      <c r="G42" s="18">
+        <v>100.023346</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>2</v>
+      </c>
+      <c r="B43" s="9">
+        <v>41</v>
+      </c>
+      <c r="C43" s="24">
+        <v>23</v>
+      </c>
+      <c r="D43" s="24">
+        <v>19</v>
+      </c>
+      <c r="E43" s="24">
+        <v>0</v>
+      </c>
+      <c r="F43" s="18">
+        <v>10.013496</v>
+      </c>
+      <c r="G43" s="18">
+        <v>100.00082</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,17 +3286,349 @@
         <v>12</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>2</v>
+      </c>
+      <c r="B39" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>2</v>
+      </c>
+      <c r="B41" s="9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>2</v>
+      </c>
+      <c r="B43" s="9">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2078,10 +3637,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,42 +3672,50 @@
         <v>12</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="14" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0</v>
+      </c>
       <c r="D2" s="15"/>
-      <c r="E2" s="19"/>
+      <c r="E2" s="19">
+        <v>38019.54</v>
+      </c>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -2156,6 +3723,580 @@
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
       <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="18">
+        <v>21367.921999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="18">
+        <v>19504.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18">
+        <v>23538.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18">
+        <v>25549.965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18">
+        <v>18225.298999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="18">
+        <v>44801.733999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
+        <v>32318.828000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="18">
+        <v>21845.942999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18">
+        <v>23653.833999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <v>14510.630999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="E13" s="18">
+        <v>57845.347999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>19121.928</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18">
+        <v>36272.332000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18">
+        <v>20972.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18">
+        <v>30607.166000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="E18" s="18">
+        <v>16582.588</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9">
+        <v>17</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0</v>
+      </c>
+      <c r="E19" s="18">
+        <v>4983.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9">
+        <v>18</v>
+      </c>
+      <c r="C20" s="16">
+        <v>0</v>
+      </c>
+      <c r="E20" s="18">
+        <v>29738.645</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9">
+        <v>19</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0</v>
+      </c>
+      <c r="E21" s="18">
+        <v>30614.799999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="9">
+        <v>20</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0</v>
+      </c>
+      <c r="E22" s="18">
+        <v>8969.7860000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="9">
+        <v>21</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0</v>
+      </c>
+      <c r="E23" s="18">
+        <v>11205.536</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9">
+        <v>22</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="18">
+        <v>39585.366999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="9">
+        <v>23</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18">
+        <v>36292.703000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="9">
+        <v>24</v>
+      </c>
+      <c r="C26" s="16">
+        <v>0</v>
+      </c>
+      <c r="E26" s="18">
+        <v>12254.038</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9">
+        <v>25</v>
+      </c>
+      <c r="C27" s="16">
+        <v>0</v>
+      </c>
+      <c r="E27" s="18">
+        <v>21970.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="9">
+        <v>26</v>
+      </c>
+      <c r="C28" s="16">
+        <v>0</v>
+      </c>
+      <c r="E28" s="18">
+        <v>24825.482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9">
+        <v>27</v>
+      </c>
+      <c r="C29" s="16">
+        <v>0</v>
+      </c>
+      <c r="E29" s="18">
+        <v>24612.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="9">
+        <v>28</v>
+      </c>
+      <c r="C30" s="16">
+        <v>0</v>
+      </c>
+      <c r="E30" s="18">
+        <v>4996.5736999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="9">
+        <v>29</v>
+      </c>
+      <c r="C31" s="16">
+        <v>0</v>
+      </c>
+      <c r="E31" s="18">
+        <v>40760.292999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="9">
+        <v>30</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0</v>
+      </c>
+      <c r="E32" s="18">
+        <v>16408.063999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="9">
+        <v>31</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0</v>
+      </c>
+      <c r="E33" s="18">
+        <v>22134.030999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="9">
+        <v>32</v>
+      </c>
+      <c r="C34" s="16">
+        <v>0</v>
+      </c>
+      <c r="E34" s="18">
+        <v>31009.998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="9">
+        <v>33</v>
+      </c>
+      <c r="C35" s="16">
+        <v>0</v>
+      </c>
+      <c r="E35" s="18">
+        <v>2249.9083999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9">
+        <v>34</v>
+      </c>
+      <c r="C36" s="16">
+        <v>0</v>
+      </c>
+      <c r="E36" s="18">
+        <v>35502.273000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="9">
+        <v>35</v>
+      </c>
+      <c r="C37" s="16">
+        <v>0</v>
+      </c>
+      <c r="E37" s="18">
+        <v>31754.195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="9">
+        <v>36</v>
+      </c>
+      <c r="C38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="18">
+        <v>30035.896000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>2</v>
+      </c>
+      <c r="B39" s="9">
+        <v>37</v>
+      </c>
+      <c r="C39" s="16">
+        <v>0</v>
+      </c>
+      <c r="E39" s="18">
+        <v>10479.474</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="9">
+        <v>38</v>
+      </c>
+      <c r="C40" s="16">
+        <v>0</v>
+      </c>
+      <c r="E40" s="18">
+        <v>13557.04</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>2</v>
+      </c>
+      <c r="B41" s="9">
+        <v>39</v>
+      </c>
+      <c r="C41" s="16">
+        <v>0</v>
+      </c>
+      <c r="E41" s="18">
+        <v>12892.931</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9">
+        <v>40</v>
+      </c>
+      <c r="C42" s="16">
+        <v>0</v>
+      </c>
+      <c r="E42" s="18">
+        <v>18479.219000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>2</v>
+      </c>
+      <c r="B43" s="9">
+        <v>41</v>
+      </c>
+      <c r="C43" s="16">
+        <v>0</v>
+      </c>
+      <c r="E43" s="18">
+        <v>13691.017</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2188,16 +4329,16 @@
         <v>12</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2239,16 +4380,16 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,49 +4448,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2404,37 +4545,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>